<commit_message>
added react with js
</commit_message>
<xml_diff>
--- a/trackcoder.xlsx
+++ b/trackcoder.xlsx
@@ -464,7 +464,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4568,7 +4568,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="103" ht="16.5" customHeight="1">
+    <row r="103" ht="19.5" customHeight="1">
       <c r="A103" s="9" t="inlineStr">
         <is>
           <t>2025-02-22</t>
@@ -4608,18 +4608,18 @@
         <v>163</v>
       </c>
     </row>
-    <row r="104" ht="16.5" customHeight="1">
+    <row r="104" ht="19.5" customHeight="1">
       <c r="A104" s="9" t="inlineStr">
         <is>
           <t>2025-02-24</t>
         </is>
       </c>
-      <c r="B104" s="6" t="inlineStr">
+      <c r="B104" s="2" t="inlineStr">
         <is>
           <t>9:45</t>
         </is>
       </c>
-      <c r="C104" s="7" t="n">
+      <c r="C104" s="3" t="n">
         <v>38</v>
       </c>
       <c r="D104" s="9" t="inlineStr">
@@ -4648,18 +4648,18 @@
         <v>164</v>
       </c>
     </row>
-    <row r="105" ht="16.5" customHeight="1">
+    <row r="105" ht="19.5" customHeight="1">
       <c r="A105" s="9" t="inlineStr">
         <is>
           <t>2025-02-25</t>
         </is>
       </c>
-      <c r="B105" s="10" t="inlineStr">
+      <c r="B105" s="2" t="inlineStr">
         <is>
           <t>2:30</t>
         </is>
       </c>
-      <c r="C105" s="10" t="n">
+      <c r="C105" s="3" t="n">
         <v>38</v>
       </c>
       <c r="D105" s="9" t="inlineStr">
@@ -4672,60 +4672,508 @@
           <t>0:52</t>
         </is>
       </c>
-      <c r="F105" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G105" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H105" s="7" t="n">
+      <c r="F105" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="I105" s="7" t="n">
+      <c r="I105" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="J105" s="7" t="n">
+      <c r="J105" s="3" t="n">
         <v>165</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
+    <row r="106" ht="19.5" customHeight="1">
+      <c r="A106" s="9" t="inlineStr">
         <is>
           <t>2025-02-26</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B106" s="2" t="inlineStr">
         <is>
           <t>8:30</t>
         </is>
       </c>
-      <c r="C106" t="n">
+      <c r="C106" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="D106" t="inlineStr">
+      <c r="D106" s="9" t="inlineStr">
         <is>
           <t>4:51</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr">
+      <c r="E106" s="9" t="inlineStr">
         <is>
           <t>3:41</t>
         </is>
       </c>
-      <c r="F106" t="n">
-        <v>0</v>
-      </c>
-      <c r="G106" t="n">
-        <v>0</v>
-      </c>
-      <c r="H106" t="n">
-        <v>109</v>
-      </c>
-      <c r="I106" t="n">
-        <v>109</v>
-      </c>
-      <c r="J106" t="n">
+      <c r="F106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="3" t="n">
+        <v>209</v>
+      </c>
+      <c r="I106" s="3" t="n">
+        <v>209</v>
+      </c>
+      <c r="J106" s="3" t="n">
         <v>166</v>
+      </c>
+    </row>
+    <row r="107" ht="16.5" customHeight="1">
+      <c r="A107" s="9" t="inlineStr">
+        <is>
+          <t>2025-02-27</t>
+        </is>
+      </c>
+      <c r="B107" s="2" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D107" s="9" t="inlineStr">
+        <is>
+          <t>7:45</t>
+        </is>
+      </c>
+      <c r="E107" s="9" t="inlineStr">
+        <is>
+          <t>5:37</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>188</v>
+      </c>
+      <c r="I107" s="3" t="n">
+        <v>196</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" ht="16.5" customHeight="1">
+      <c r="A108" s="9" t="inlineStr">
+        <is>
+          <t>2025-02-28</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="inlineStr">
+        <is>
+          <t>10:20</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D108" s="9" t="inlineStr">
+        <is>
+          <t>4:20</t>
+        </is>
+      </c>
+      <c r="E108" s="9" t="inlineStr">
+        <is>
+          <t>2:06</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>140</v>
+      </c>
+      <c r="I108" s="3" t="n">
+        <v>144</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="109" ht="16.5" customHeight="1">
+      <c r="A109" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-01</t>
+        </is>
+      </c>
+      <c r="B109" s="6" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="C109" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="D109" s="9" t="inlineStr">
+        <is>
+          <t>1:35</t>
+        </is>
+      </c>
+      <c r="E109" s="9" t="inlineStr">
+        <is>
+          <t>0:17</t>
+        </is>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="I109" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" ht="16.5" customHeight="1">
+      <c r="A110" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
+      <c r="B110" s="6" t="inlineStr">
+        <is>
+          <t>8:41</t>
+        </is>
+      </c>
+      <c r="C110" s="7" t="n">
+        <v>39</v>
+      </c>
+      <c r="D110" s="9" t="inlineStr">
+        <is>
+          <t>3:41</t>
+        </is>
+      </c>
+      <c r="E110" s="9" t="inlineStr">
+        <is>
+          <t>0:56</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I110" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" ht="16.5" customHeight="1">
+      <c r="A111" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-04</t>
+        </is>
+      </c>
+      <c r="B111" s="10" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="C111" s="10" t="n">
+        <v>41</v>
+      </c>
+      <c r="D111" s="9" t="inlineStr">
+        <is>
+          <t>3:35</t>
+        </is>
+      </c>
+      <c r="E111" s="9" t="inlineStr">
+        <is>
+          <t>0:52</t>
+        </is>
+      </c>
+      <c r="F111" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="I111" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="J111" s="7" t="n">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" ht="16.5" customHeight="1">
+      <c r="A112" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B112" s="10" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C112" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="D112" s="9" t="inlineStr">
+        <is>
+          <t>5:24</t>
+        </is>
+      </c>
+      <c r="E112" s="9" t="inlineStr">
+        <is>
+          <t>2:36</t>
+        </is>
+      </c>
+      <c r="F112" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="I112" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="J112" s="7" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="113" ht="16.5" customHeight="1">
+      <c r="A113" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-06</t>
+        </is>
+      </c>
+      <c r="B113" s="10" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C113" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="D113" s="9" t="inlineStr">
+        <is>
+          <t>5:24</t>
+        </is>
+      </c>
+      <c r="E113" s="9" t="inlineStr">
+        <is>
+          <t>2:46</t>
+        </is>
+      </c>
+      <c r="F113" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" s="7" t="n">
+        <v>208</v>
+      </c>
+      <c r="I113" s="7" t="n">
+        <v>208</v>
+      </c>
+      <c r="J113" s="7" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>6:58</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>5:58</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>3:42</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>113</v>
+      </c>
+      <c r="I114" t="n">
+        <v>113</v>
+      </c>
+      <c r="J114" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>7:27</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>6:27</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0:14</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-03-10</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>6:39</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>4:15</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" t="n">
+        <v>228</v>
+      </c>
+      <c r="I116" t="n">
+        <v>228</v>
+      </c>
+      <c r="J116" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>5:22</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2:32</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" t="n">
+        <v>164</v>
+      </c>
+      <c r="I117" t="n">
+        <v>165</v>
+      </c>
+      <c r="J117" t="n">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add documentation for Track_Coder project
</commit_message>
<xml_diff>
--- a/trackcoder.xlsx
+++ b/trackcoder.xlsx
@@ -464,7 +464,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,7 +474,7 @@
   <cols>
     <col width="15.71928571428571" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
     <col width="9.147857142857141" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
-    <col width="11.86214285714286" bestFit="1" customWidth="1" style="10" min="3" max="3"/>
+    <col width="11.86214285714286" bestFit="1" customWidth="1" style="11" min="3" max="3"/>
     <col width="9.147857142857141" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
     <col width="9.147857142857141" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
     <col width="11.86214285714286" bestFit="1" customWidth="1" style="11" min="6" max="6"/>
@@ -4728,7 +4728,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="107" ht="16.5" customHeight="1">
+    <row r="107" ht="19.5" customHeight="1">
       <c r="A107" s="9" t="inlineStr">
         <is>
           <t>2025-02-27</t>
@@ -4768,7 +4768,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="108" ht="16.5" customHeight="1">
+    <row r="108" ht="19.5" customHeight="1">
       <c r="A108" s="9" t="inlineStr">
         <is>
           <t>2025-02-28</t>
@@ -4808,18 +4808,18 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109" ht="16.5" customHeight="1">
+    <row r="109" ht="19.5" customHeight="1">
       <c r="A109" s="9" t="inlineStr">
         <is>
           <t>2025-03-01</t>
         </is>
       </c>
-      <c r="B109" s="6" t="inlineStr">
+      <c r="B109" s="2" t="inlineStr">
         <is>
           <t>9:00</t>
         </is>
       </c>
-      <c r="C109" s="7" t="n">
+      <c r="C109" s="3" t="n">
         <v>37</v>
       </c>
       <c r="D109" s="9" t="inlineStr">
@@ -4848,18 +4848,18 @@
         <v>169</v>
       </c>
     </row>
-    <row r="110" ht="16.5" customHeight="1">
+    <row r="110" ht="19.5" customHeight="1">
       <c r="A110" s="9" t="inlineStr">
         <is>
           <t>2025-03-03</t>
         </is>
       </c>
-      <c r="B110" s="6" t="inlineStr">
+      <c r="B110" s="2" t="inlineStr">
         <is>
           <t>8:41</t>
         </is>
       </c>
-      <c r="C110" s="7" t="n">
+      <c r="C110" s="3" t="n">
         <v>39</v>
       </c>
       <c r="D110" s="9" t="inlineStr">
@@ -4888,18 +4888,18 @@
         <v>170</v>
       </c>
     </row>
-    <row r="111" ht="16.5" customHeight="1">
+    <row r="111" ht="19.5" customHeight="1">
       <c r="A111" s="9" t="inlineStr">
         <is>
           <t>2025-03-04</t>
         </is>
       </c>
-      <c r="B111" s="10" t="inlineStr">
+      <c r="B111" s="2" t="inlineStr">
         <is>
           <t>9:00</t>
         </is>
       </c>
-      <c r="C111" s="10" t="n">
+      <c r="C111" s="3" t="n">
         <v>41</v>
       </c>
       <c r="D111" s="9" t="inlineStr">
@@ -4912,34 +4912,34 @@
           <t>0:52</t>
         </is>
       </c>
-      <c r="F111" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H111" s="7" t="n">
+      <c r="F111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="I111" s="7" t="n">
+      <c r="I111" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="J111" s="7" t="n">
+      <c r="J111" s="3" t="n">
         <v>171</v>
       </c>
     </row>
-    <row r="112" ht="16.5" customHeight="1">
+    <row r="112" ht="19.5" customHeight="1">
       <c r="A112" s="9" t="inlineStr">
         <is>
           <t>2025-03-05</t>
         </is>
       </c>
-      <c r="B112" s="10" t="inlineStr">
+      <c r="B112" s="2" t="inlineStr">
         <is>
           <t>8:30</t>
         </is>
       </c>
-      <c r="C112" s="10" t="n">
+      <c r="C112" s="3" t="n">
         <v>44</v>
       </c>
       <c r="D112" s="9" t="inlineStr">
@@ -4952,34 +4952,34 @@
           <t>2:36</t>
         </is>
       </c>
-      <c r="F112" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G112" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H112" s="7" t="n">
+      <c r="F112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="I112" s="7" t="n">
+      <c r="I112" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="J112" s="7" t="n">
+      <c r="J112" s="3" t="n">
         <v>172</v>
       </c>
     </row>
-    <row r="113" ht="16.5" customHeight="1">
+    <row r="113" ht="19.5" customHeight="1">
       <c r="A113" s="9" t="inlineStr">
         <is>
           <t>2025-03-06</t>
         </is>
       </c>
-      <c r="B113" s="10" t="inlineStr">
+      <c r="B113" s="2" t="inlineStr">
         <is>
           <t>8:30</t>
         </is>
       </c>
-      <c r="C113" s="10" t="n">
+      <c r="C113" s="3" t="n">
         <v>42</v>
       </c>
       <c r="D113" s="9" t="inlineStr">
@@ -4992,188 +4992,386 @@
           <t>2:46</t>
         </is>
       </c>
-      <c r="F113" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G113" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H113" s="7" t="n">
+      <c r="F113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" s="3" t="n">
         <v>208</v>
       </c>
-      <c r="I113" s="7" t="n">
+      <c r="I113" s="3" t="n">
         <v>208</v>
       </c>
-      <c r="J113" s="7" t="n">
+      <c r="J113" s="3" t="n">
         <v>173</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
+    <row r="114" ht="19.5" customHeight="1">
+      <c r="A114" s="9" t="inlineStr">
         <is>
           <t>2025-03-07</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
+      <c r="B114" s="2" t="inlineStr">
         <is>
           <t>6:58</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
+      <c r="C114" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D114" s="9" t="inlineStr">
         <is>
           <t>5:58</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr">
+      <c r="E114" s="9" t="inlineStr">
         <is>
           <t>3:42</t>
         </is>
       </c>
-      <c r="F114" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="n">
-        <v>0</v>
-      </c>
-      <c r="H114" t="n">
+      <c r="F114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="I114" t="n">
+      <c r="I114" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="J114" t="n">
+      <c r="J114" s="3" t="n">
         <v>174</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
+    <row r="115" ht="19.5" customHeight="1">
+      <c r="A115" s="9" t="inlineStr">
         <is>
           <t>2025-03-09</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
+      <c r="B115" s="2" t="inlineStr">
         <is>
           <t>7:27</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
+      <c r="C115" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D115" s="9" t="inlineStr">
         <is>
           <t>6:27</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr">
+      <c r="E115" s="9" t="inlineStr">
         <is>
           <t>0:14</t>
         </is>
       </c>
-      <c r="F115" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" t="n">
-        <v>0</v>
-      </c>
-      <c r="H115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I115" t="n">
-        <v>0</v>
-      </c>
-      <c r="J115" t="n">
+      <c r="F115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" s="3" t="n">
         <v>175</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
+    <row r="116" ht="16.5" customHeight="1">
+      <c r="A116" s="9" t="inlineStr">
         <is>
           <t>2025-03-10</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B116" s="2" t="inlineStr">
         <is>
           <t>8:30</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
+      <c r="C116" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D116" s="9" t="inlineStr">
         <is>
           <t>6:39</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="E116" s="9" t="inlineStr">
         <is>
           <t>4:15</t>
         </is>
       </c>
-      <c r="F116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G116" t="n">
-        <v>0</v>
-      </c>
-      <c r="H116" t="n">
+      <c r="F116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="3" t="n">
         <v>228</v>
       </c>
-      <c r="I116" t="n">
+      <c r="I116" s="3" t="n">
         <v>228</v>
       </c>
-      <c r="J116" t="n">
+      <c r="J116" s="3" t="n">
         <v>176</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
+    <row r="117" ht="16.5" customHeight="1">
+      <c r="A117" s="9" t="inlineStr">
         <is>
           <t>2025-03-11</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
+      <c r="B117" s="2" t="inlineStr">
         <is>
           <t>8:00</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
+      <c r="C117" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="D117" s="9" t="inlineStr">
         <is>
           <t>5:22</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
+      <c r="E117" s="9" t="inlineStr">
         <is>
           <t>2:32</t>
         </is>
       </c>
-      <c r="F117" t="n">
+      <c r="F117" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G117" t="n">
-        <v>0</v>
-      </c>
-      <c r="H117" t="n">
-        <v>164</v>
-      </c>
-      <c r="I117" t="n">
+      <c r="G117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>264</v>
+      </c>
+      <c r="I117" s="3" t="n">
+        <v>265</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="118" ht="16.5" customHeight="1">
+      <c r="A118" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="B118" s="6" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="C118" s="7" t="n">
+        <v>47</v>
+      </c>
+      <c r="D118" s="9" t="inlineStr">
+        <is>
+          <t>6:11</t>
+        </is>
+      </c>
+      <c r="E118" s="9" t="inlineStr">
+        <is>
+          <t>4:07</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="I118" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="J118" s="3" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="119" ht="16.5" customHeight="1">
+      <c r="A119" s="9" t="inlineStr">
+        <is>
+          <t>2025-03-14</t>
+        </is>
+      </c>
+      <c r="B119" s="10" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C119" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D119" s="9" t="inlineStr">
+        <is>
+          <t>3:23</t>
+        </is>
+      </c>
+      <c r="E119" s="9" t="inlineStr">
+        <is>
+          <t>0:20</t>
+        </is>
+      </c>
+      <c r="F119" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="I119" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="J119" s="7" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-03-15</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>5:34</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>1:48</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>64</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" t="n">
+        <v>4</v>
+      </c>
+      <c r="I120" t="n">
+        <v>68</v>
+      </c>
+      <c r="J120" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>4:33</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>13</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>152</v>
+      </c>
+      <c r="I121" t="n">
         <v>165</v>
       </c>
-      <c r="J117" t="n">
-        <v>177</v>
+      <c r="J121" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-03-19</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>4:02</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>1:40</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>37</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="n">
+        <v>40</v>
+      </c>
+      <c r="I122" t="n">
+        <v>77</v>
+      </c>
+      <c r="J122" t="n">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>